<commit_message>
applied oops to dynamically change ranks along with houses and its logos
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Event</t>
   </si>
@@ -41,6 +41,13 @@
   </si>
   <si>
     <t>pitthu</t>
+  </si>
+  <si>
+    <t>Inpromptu Rapid
+Fire</t>
+  </si>
+  <si>
+    <t>Chess</t>
   </si>
   <si>
     <t>total</t>
@@ -50,7 +57,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -62,6 +69,11 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -71,18 +83,61 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border/>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,24 +458,82 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
+    <row r="7">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="B7" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="8">
+        <v>28.0</v>
+      </c>
+      <c r="C9" s="8">
+        <v>17.0</v>
+      </c>
+      <c r="D9" s="8">
+        <v>18.0</v>
+      </c>
+      <c r="E9" s="8">
         <v>14.0</v>
       </c>
-      <c r="D11" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>12.0</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G7:H7"/>
+  </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>

</xml_diff>